<commit_message>
excel updates with data
</commit_message>
<xml_diff>
--- a/analytics/campgrounds.xlsx
+++ b/analytics/campgrounds.xlsx
@@ -1,107 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CampQuest\CampQuest\analytics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BD9930-E239-42A2-B857-509ED28DAD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Campgrounds" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Rating</t>
-  </si>
-  <si>
-    <t>Maple Hunting Camp</t>
-  </si>
-  <si>
-    <t>Bethlehem, Pennsylvania</t>
-  </si>
-  <si>
-    <t>Elk Bay</t>
-  </si>
-  <si>
-    <t>Tamarac, Florida</t>
-  </si>
-  <si>
-    <t>Ocean Bay</t>
-  </si>
-  <si>
-    <t>Charleston, South Carolina</t>
-  </si>
-  <si>
-    <t>Maple Creekside</t>
-  </si>
-  <si>
-    <t>Parker, Colorado</t>
-  </si>
-  <si>
-    <t>Sea Hollow</t>
-  </si>
-  <si>
-    <t>Brockton, Massachusetts</t>
-  </si>
-  <si>
-    <t>Ancient Bay</t>
-  </si>
-  <si>
-    <t>Gresham, Oregon</t>
-  </si>
-  <si>
-    <t>Diamond Bayshore</t>
-  </si>
-  <si>
-    <t>Torrance, California</t>
-  </si>
-  <si>
-    <t>Petrified Pond</t>
-  </si>
-  <si>
-    <t>Wyoming, Michigan</t>
-  </si>
-  <si>
-    <t>Redwood Village</t>
-  </si>
-  <si>
-    <t>Waterloo, Iowa</t>
-  </si>
-  <si>
-    <t>Dusty Hollow</t>
-  </si>
-  <si>
-    <t>Albany, Oregon</t>
-  </si>
-  <si>
-    <t>Rushabh's FarmHouse</t>
-  </si>
-  <si>
-    <t>Surat, India</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -470,154 +396,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.09765625" customWidth="1"/>
-    <col min="2" max="2" width="22.8984375" customWidth="1"/>
-    <col min="3" max="3" width="21.09765625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Location</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Rating</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Elk Bay</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Tamarac, Florida</v>
+      </c>
+      <c r="C2">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Ocean Bay</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Charleston, South Carolina</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Maple Creekside</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Parker, Colorado</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Sea Hollow</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Brockton, Massachusetts</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Ancient Bay</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Gresham, Oregon</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Diamond Bayshore</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Torrance, California</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Petrified Pond</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Wyoming, Michigan</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Redwood Village</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Waterloo, Iowa</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Dusty Hollow</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Albany, Oregon</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Rushabh's FarmHouse</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Surat, India</v>
       </c>
       <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C12" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added analytic, project finished 13/10/2024
</commit_message>
<xml_diff>
--- a/analytics/campgrounds.xlsx
+++ b/analytics/campgrounds.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -426,32 +426,32 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Ocean Bay</v>
+        <v>Camp2</v>
       </c>
       <c r="B3" t="str">
-        <v>Charleston, South Carolina</v>
+        <v>Tamarac, Florida</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Maple Creekside</v>
+        <v>Rushabh's FarmHouse</v>
       </c>
       <c r="B4" t="str">
-        <v>Parker, Colorado</v>
+        <v>Surat, India</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Sea Hollow</v>
+        <v>Ocean Bay</v>
       </c>
       <c r="B5" t="str">
-        <v>Brockton, Massachusetts</v>
+        <v>Charleston, South Carolina</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -459,10 +459,10 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Ancient Bay</v>
+        <v>Maple Creekside</v>
       </c>
       <c r="B6" t="str">
-        <v>Gresham, Oregon</v>
+        <v>Parker, Colorado</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -470,10 +470,10 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Diamond Bayshore</v>
+        <v>Sea Hollow</v>
       </c>
       <c r="B7" t="str">
-        <v>Torrance, California</v>
+        <v>Brockton, Massachusetts</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Petrified Pond</v>
+        <v>Ancient Bay</v>
       </c>
       <c r="B8" t="str">
-        <v>Wyoming, Michigan</v>
+        <v>Gresham, Oregon</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -492,10 +492,10 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Redwood Village</v>
+        <v>Diamond Bayshore</v>
       </c>
       <c r="B9" t="str">
-        <v>Waterloo, Iowa</v>
+        <v>Torrance, California</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -503,10 +503,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Dusty Hollow</v>
+        <v>Petrified Pond</v>
       </c>
       <c r="B10" t="str">
-        <v>Albany, Oregon</v>
+        <v>Wyoming, Michigan</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -514,18 +514,51 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Rushabh's FarmHouse</v>
+        <v>Redwood Village</v>
       </c>
       <c r="B11" t="str">
-        <v>Surat, India</v>
+        <v>Waterloo, Iowa</v>
       </c>
       <c r="C11">
-        <v>3.5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Dusty Hollow</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Albany, Oregon</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Camp2</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Tamarac, Florida</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Camp2</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Tamarac, Florida</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated gitignore to exclude campgrounds.xlsx
</commit_message>
<xml_diff>
--- a/analytics/campgrounds.xlsx
+++ b/analytics/campgrounds.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,18 +415,18 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Elk Bay</v>
+        <v>Diamond Bayshore</v>
       </c>
       <c r="B2" t="str">
-        <v>Tamarac, Florida</v>
+        <v>Torrance, California</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Camp2</v>
+        <v>Elk Bay</v>
       </c>
       <c r="B3" t="str">
         <v>Tamarac, Florida</v>
@@ -437,32 +437,32 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Rushabh's FarmHouse</v>
+        <v>Camp2</v>
       </c>
       <c r="B4" t="str">
-        <v>Surat, India</v>
+        <v>Tamarac, Florida</v>
       </c>
       <c r="C4">
-        <v>3.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Ocean Bay</v>
+        <v>Nature's FarmHouse</v>
       </c>
       <c r="B5" t="str">
-        <v>Charleston, South Carolina</v>
+        <v>Surat, India</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Maple Creekside</v>
+        <v>Ocean Bay</v>
       </c>
       <c r="B6" t="str">
-        <v>Parker, Colorado</v>
+        <v>Charleston, South Carolina</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -470,10 +470,10 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Sea Hollow</v>
+        <v>Maple Creekside</v>
       </c>
       <c r="B7" t="str">
-        <v>Brockton, Massachusetts</v>
+        <v>Parker, Colorado</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Ancient Bay</v>
+        <v>Sea Hollow</v>
       </c>
       <c r="B8" t="str">
-        <v>Gresham, Oregon</v>
+        <v>Brockton, Massachusetts</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -492,10 +492,10 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Diamond Bayshore</v>
+        <v>Ancient Bay</v>
       </c>
       <c r="B9" t="str">
-        <v>Torrance, California</v>
+        <v>Gresham, Oregon</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -556,9 +556,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Safal Ganga</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Chenbur Colony, Chembur</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>